<commit_message>
Service name loader from OPENMRS task done, and UUID matching implemented for amount fetching
</commit_message>
<xml_diff>
--- a/build/assets/files/Services.xlsx
+++ b/build/assets/files/Services.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\MOH OTC VERSIONS\MOH_OTC_hospital_later_version\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B92436E-B147-4733-A341-762B417924E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026DCAB8-C250-4306-A00F-68AC50A5C8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1FD553E2-D7F1-4E34-B132-48A70073EE8C}"/>
   </bookViews>
@@ -25,12 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Services</t>
+    <t>ShortCode</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>SubGroup</t>
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -114,11 +123,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E4DD12E-BF14-43A4-A639-9A09673F1007}" name="Table1" displayName="Table1" ref="A1:B2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B2" xr:uid="{4E4DD12E-BF14-43A4-A639-9A09673F1007}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{42C4E1B0-D08F-4643-B3C7-C0A1AE4ED22D}" name="Services"/>
-    <tableColumn id="2" xr3:uid="{E330F4A9-598D-4180-9538-58D88B218A73}" name="Amount"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E4DD12E-BF14-43A4-A639-9A09673F1007}" name="Table1" displayName="Table1" ref="A1:E2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E2" xr:uid="{4E4DD12E-BF14-43A4-A639-9A09673F1007}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{42C4E1B0-D08F-4643-B3C7-C0A1AE4ED22D}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{E330F4A9-598D-4180-9538-58D88B218A73}" name="ShortCode"/>
+    <tableColumn id="3" xr3:uid="{87B7DD6A-6C80-490A-8AD5-B36E37A22272}" name="Group"/>
+    <tableColumn id="4" xr3:uid="{BFD3E820-0028-487D-A452-1A981AA89470}" name="SubGroup"/>
+    <tableColumn id="5" xr3:uid="{CD13DB7B-B1D4-46ED-B7B6-141B6C86CC36}" name="Amount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -421,24 +433,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEB2173-902F-4629-8891-85050C9F2D2C}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>